<commit_message>
Updated Design Document for Sprint 3
</commit_message>
<xml_diff>
--- a/docs/CS180 5J's JBox Design Document.xlsx
+++ b/docs/CS180 5J's JBox Design Document.xlsx
@@ -201,7 +201,7 @@
 3. Player controls of play, pause, skip is hidden from users and only Host can see.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A14">
+    <comment authorId="0" ref="B14">
       <text>
         <t xml:space="preserve">Accepting criteria:
 1. UI displays the Song status (playing paused etc) for all users
@@ -209,20 +209,20 @@
 3. Player controls of play, pause, skip is hidden from users and only Host can see.</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A15">
+    <comment authorId="0" ref="B15">
       <text>
         <t xml:space="preserve">Acceptance Criteria:
 1) Host and uses should be able to see number of people currently in the room</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A16">
+    <comment authorId="0" ref="B16">
       <text>
         <t xml:space="preserve">Acceptance criteria:
 1. Users are able to vote to have a song repeated
 2. Host is able to repeat songs with impunity</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A17">
+    <comment authorId="0" ref="B17">
       <text>
         <t xml:space="preserve">Accepting criteria
 1. Host has a button that allows or forbid duplicate songs in the queue
@@ -230,7 +230,7 @@
 3. When it is not vice versa</t>
       </text>
     </comment>
-    <comment authorId="0" ref="A18">
+    <comment authorId="0" ref="B18">
       <text>
         <t xml:space="preserve">Accepting Criteria:
 1. Users are able to vote to remove any visible songs in the queue
@@ -347,13 +347,34 @@
     <t>Done</t>
   </si>
   <si>
+    <t>Story Points</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Task 1: Create basic interface for the main page, with CreateRoom and JoinRoom button. (Enoch)</t>
+  </si>
+  <si>
     <t>Author</t>
   </si>
   <si>
     <t>Jae Hyun Yim, Justin Yoo, Jang-Shing Lin, Jiawei Chen, Justin Li</t>
   </si>
   <si>
-    <t>Task 1: Create basic interface for the main page, with CreateRoom and JoinRoom button. (Enoch)</t>
+    <t>Task 2: CreateRoom button creates a new room page and displays song status (Justin Li, Jiawei Chen)</t>
+  </si>
+  <si>
+    <t>Task 3: The new room page is then connected to spotify account API. (Jae)</t>
+  </si>
+  <si>
+    <t>Task 4: Generate unique code for room access (Justin Y)</t>
+  </si>
+  <si>
+    <t>Task 5: Users can access the room page with the unique code. (Justin Yoo)</t>
   </si>
   <si>
     <t>Email</t>
@@ -362,73 +383,70 @@
     <t>jyim008@ucr.edu, jyoo030@ucr.edu, jchen313@ucr.edu, lli109@ucr.edu, jlin065@ucr.edu</t>
   </si>
   <si>
-    <t>Task 2: CreateRoom button creates a new room page and displays song status (Justin Li, Jiawei Chen)</t>
-  </si>
-  <si>
-    <t>Task 3: The new room page is then connected to spotify account API. (Jae)</t>
+    <t>Task 6: a host or user is able to be able to search for songs using the Spotify API. (Justin yoo)</t>
+  </si>
+  <si>
+    <t>Host rooms</t>
+  </si>
+  <si>
+    <t>Task 7: a host or user is able to add songs to the queue. (Jae)</t>
+  </si>
+  <si>
+    <t>Task 8: a host is be able add or remove songs from the queue, and play and skip. (Jae)</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Task 4: Generate unique code for room access (Justin Y)</t>
-  </si>
-  <si>
-    <t>Task 5: Users can access the room page with the unique code. (Justin Yoo)</t>
-  </si>
-  <si>
-    <t>Task 6: a host or user is able to be able to search for songs using the Spotify API. (Justin yoo)</t>
-  </si>
-  <si>
-    <t>Task 7: a host or user is able to add songs to the queue. (Jae)</t>
-  </si>
-  <si>
-    <t>Story Points</t>
-  </si>
-  <si>
-    <t>Task 8: a host is be able add or remove songs from the queue, and play and skip. (Jae)</t>
-  </si>
-  <si>
-    <t>Priority</t>
-  </si>
-  <si>
-    <t>Comments</t>
+    <t>Task 9: Reconcile React code with ejs/bootstrap (Enoch, Jiawei, Justin Li)</t>
   </si>
   <si>
     <t>Spotify website version (Modified version)</t>
   </si>
   <si>
-    <t>Host rooms</t>
-  </si>
-  <si>
-    <t>Task 9: Reconcile React code with ejs/bootstrap (Enoch, Jiawei, Justin Li)</t>
-  </si>
-  <si>
     <t>Task 10: a user should be able to see current song playing, next songs, and the player. (Backend)</t>
   </si>
   <si>
+    <t>Tabs</t>
+  </si>
+  <si>
     <t>As a user I want to create a room with a unique room ID that give to other users so they can join my room. I become the host.</t>
   </si>
   <si>
-    <t>Task 11: a user should be able to see current song playing, next songs, and the player. (Frontend) (Jiawei)</t>
-  </si>
-  <si>
-    <t>Task 12: a host or user should be able to see number of users currently in the room(Justin Li)</t>
-  </si>
-  <si>
-    <t>Tabs</t>
-  </si>
-  <si>
-    <t>Task 13: As a user I should be able to repeat songs.</t>
+    <t>Task 11: a user should be able to see current song playing, next songs, and the player. (Frontend) (Jiawei, Enoch)</t>
+  </si>
+  <si>
+    <t>Task 12: a host or user should be able to see number of users currently in the room(Justin Li, Enoch)</t>
   </si>
   <si>
     <t>Join rooms</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Task 13: As a user I should be able to repeat songs. (Justin Li, Jae)</t>
+  </si>
+  <si>
     <t>I want to be able to use a unique room ID to join another users room.</t>
   </si>
   <si>
-    <t>Notes</t>
+    <t>"Product Backlog"</t>
+  </si>
+  <si>
+    <t>Task 14: As a host I should be able to decide if duplicates are added to the queue. (Justin Li, Jae)</t>
+  </si>
+  <si>
+    <t>Task 15: As a user I should be able to vote on whether to remove/skip the current and next songs. (Justin Yoo, Jiawei)</t>
+  </si>
+  <si>
+    <t>Should be initialized with the user stories and their estimated efforts (i.e., story points)</t>
+  </si>
+  <si>
+    <t>Depending on the amount of story points, some stories may need to be split into smaller stories</t>
+  </si>
+  <si>
+    <t>Add "Acceptance Criteria" to each user story by "insert note" to a spreadsheet cell (right click the cell)</t>
   </si>
   <si>
     <t>Add to queue</t>
@@ -437,10 +455,7 @@
     <t>As a host or user I want to be able to add songs to the queue.</t>
   </si>
   <si>
-    <t>"Product Backlog"</t>
-  </si>
-  <si>
-    <t>Should be initialized with the user stories and their estimated efforts (i.e., story points)</t>
+    <t>"Acceptance Criteria" define what it means by "Done"</t>
   </si>
   <si>
     <t>Host controls</t>
@@ -449,35 +464,56 @@
     <t>As a host, I want to be able add or remove songs from the queue, and play and skip.</t>
   </si>
   <si>
-    <t>Depending on the amount of story points, some stories may need to be split into smaller stories</t>
-  </si>
-  <si>
-    <t>Add "Acceptance Criteria" to each user story by "insert note" to a spreadsheet cell (right click the cell)</t>
-  </si>
-  <si>
     <t>Search Songs</t>
   </si>
   <si>
     <t>As a host or user I want to be able to be able to search for songs using the Spotify API.</t>
   </si>
   <si>
-    <t>Task 14: As a host I should be able to decide if duplicates are added to the queue.</t>
-  </si>
-  <si>
-    <t>"Acceptance Criteria" define what it means by "Done"</t>
-  </si>
-  <si>
-    <t>Task 15: As a user I should be able to vote on whether to remove/skip the current and next songs.</t>
+    <t>"Task Board"</t>
+  </si>
+  <si>
+    <t>"To Do" is initialized with tasks defined during the Sprint Planning Meeting (i.e., sprint backlog)</t>
+  </si>
+  <si>
+    <t>Tasks are expected to have similar sizes, each with a time cost of roughly 3-4 hours</t>
+  </si>
+  <si>
+    <t>Add "Details" and "Acceptance Criteria" to a task by "insert note" to a spreadsheet cell (right click the cell)</t>
+  </si>
+  <si>
+    <t>Minimize task assignments at the Sprint Planning Meeting</t>
+  </si>
+  <si>
+    <t>During a sprint, members who become available can pull tasks from the "To Do" list by moving them to "In Progress" and attaching his/her name</t>
+  </si>
+  <si>
+    <t>Inform your teammates know before you pull a task from "To Do" list</t>
+  </si>
+  <si>
+    <t>"To Verify" should be pulled by a different team member; This is a good time to perform code review and unit testing</t>
+  </si>
+  <si>
+    <t>A task in "Done" list should have its verifier's name appended</t>
   </si>
   <si>
     <t>Spotify API</t>
+  </si>
+  <si>
+    <t>"Archives"</t>
+  </si>
+  <si>
+    <t>At the end of a Sprint, finished tasks are moved to "Archives"; Unfinished tasks are moved to the next Sprint Planning Meeting</t>
   </si>
   <si>
     <t>As the host of the room I want to be able to connect use my 
 Spotify Premium Account</t>
   </si>
   <si>
-    <t>"Task Board"</t>
+    <t>"Burndown Chart"</t>
+  </si>
+  <si>
+    <t>At the end of a Sprint, update the "Burndown Chart"</t>
   </si>
   <si>
     <t>Close rooms</t>
@@ -487,45 +523,12 @@
  Spotify account and kick out all the other users.</t>
   </si>
   <si>
-    <t>"To Do" is initialized with tasks defined during the Sprint Planning Meeting (i.e., sprint backlog)</t>
-  </si>
-  <si>
-    <t>Tasks are expected to have similar sizes, each with a time cost of roughly 3-4 hours</t>
-  </si>
-  <si>
-    <t>Add "Details" and "Acceptance Criteria" to a task by "insert note" to a spreadsheet cell (right click the cell)</t>
-  </si>
-  <si>
-    <t>Minimize task assignments at the Sprint Planning Meeting</t>
-  </si>
-  <si>
-    <t>During a sprint, members who become available can pull tasks from the "To Do" list by moving them to "In Progress" and attaching his/her name</t>
-  </si>
-  <si>
-    <t>Inform your teammates know before you pull a task from "To Do" list</t>
-  </si>
-  <si>
-    <t>"To Verify" should be pulled by a different team member; This is a good time to perform code review and unit testing</t>
+    <t>if "Story Points (Remaining)" is above the "Ideal", it would be an indicator for slow progress</t>
   </si>
   <si>
     <t>Song status</t>
   </si>
   <si>
-    <t>A task in "Done" list should have its verifier's name appended</t>
-  </si>
-  <si>
-    <t>"Archives"</t>
-  </si>
-  <si>
-    <t>At the end of a Sprint, finished tasks are moved to "Archives"; Unfinished tasks are moved to the next Sprint Planning Meeting</t>
-  </si>
-  <si>
-    <t>"Burndown Chart"</t>
-  </si>
-  <si>
-    <t>At the end of a Sprint, update the "Burndown Chart"</t>
-  </si>
-  <si>
     <t>As a user I should be able to see current song playing, next songs, and the player.</t>
   </si>
   <si>
@@ -533,9 +536,6 @@
   </si>
   <si>
     <t>Repeat</t>
-  </si>
-  <si>
-    <t>if "Story Points (Remaining)" is above the "Ideal", it would be an indicator for slow progress</t>
   </si>
   <si>
     <t>As a user I should be able to repeat songs.</t>
@@ -592,6 +592,9 @@
     <t>Enoch</t>
   </si>
   <si>
+    <t>Jae</t>
+  </si>
+  <si>
     <t>Story Points (Total)</t>
   </si>
   <si>
@@ -605,9 +608,6 @@
   </si>
   <si>
     <t>Ideal</t>
-  </si>
-  <si>
-    <t>Jae</t>
   </si>
 </sst>
 </file>
@@ -628,10 +628,10 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -764,92 +764,98 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -857,15 +863,9 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -875,14 +875,14 @@
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,153 +926,153 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="6">
         <v>43390.0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>9</v>
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>12</v>
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="12" t="s">
         <v>24</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="23" t="s">
+      <c r="A7" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="21"/>
-      <c r="B8" s="23" t="s">
-        <v>42</v>
+      <c r="A8" s="20"/>
+      <c r="B8" s="21" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="21"/>
-      <c r="B9" s="24" t="s">
-        <v>43</v>
+      <c r="A9" s="20"/>
+      <c r="B9" s="23" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="25"/>
-      <c r="B10" s="27" t="s">
-        <v>47</v>
+      <c r="A10" s="24"/>
+      <c r="B10" s="26" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="25"/>
-      <c r="B11" s="24"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="24"/>
+      <c r="B13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="23" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" s="24"/>
+      <c r="B14" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="24"/>
+      <c r="B15" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="24"/>
+      <c r="B16" s="26" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23" t="s">
+    <row r="17">
+      <c r="A17" s="24"/>
+      <c r="B17" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="25"/>
-      <c r="B14" s="24" t="s">
+    <row r="18">
+      <c r="A18" s="24"/>
+      <c r="B18" s="23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="25"/>
-      <c r="B15" s="23" t="s">
+    <row r="19">
+      <c r="A19" s="20"/>
+      <c r="B19" s="23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="25"/>
-      <c r="B16" s="27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="25"/>
-      <c r="B17" s="24" t="s">
+    <row r="20">
+      <c r="A20" s="20"/>
+      <c r="B20" s="23"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="25"/>
-      <c r="B18" s="24" t="s">
+      <c r="B21" s="23" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="21"/>
-      <c r="B19" s="24" t="s">
+    <row r="22">
+      <c r="A22" s="27"/>
+      <c r="B22" s="23"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="20" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="21"/>
-      <c r="B20" s="24"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="21" t="s">
+      <c r="B23" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="24" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="29"/>
-      <c r="B22" s="24"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="24" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" s="30"/>
+      <c r="B24" s="32" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="33"/>
-      <c r="B24" s="35" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1103,33 +1103,33 @@
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>1.0</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="11">
+        <v>29</v>
+      </c>
+      <c r="D2" s="9">
         <v>3.0</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="9">
         <v>1.0</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1137,19 +1137,19 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>2.0</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="11">
+        <v>32</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="9">
         <v>3.0</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="9">
         <v>5.0</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1157,19 +1157,19 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>3.0</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="11">
+        <v>42</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="9">
         <v>3.0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>9.0</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1177,19 +1177,19 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="22">
+      <c r="A5" s="25">
         <v>4.0</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="11">
+        <v>45</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="9">
         <v>4.0</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="9">
         <v>10.0</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1197,19 +1197,19 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="11">
+      <c r="A6" s="9">
         <v>5.0</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="26">
+        <v>47</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="28">
         <v>4.0</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>8.0</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -1217,19 +1217,19 @@
       </c>
     </row>
     <row r="7" ht="28.5" customHeight="1">
-      <c r="A7" s="22">
+      <c r="A7" s="25">
         <v>6.0</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="28">
+        <v>58</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="29">
         <v>8.0</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="9">
         <v>2.0</v>
       </c>
       <c r="F7" s="7" t="s">
@@ -1237,19 +1237,19 @@
       </c>
     </row>
     <row r="8" ht="27.0" customHeight="1">
-      <c r="A8" s="11">
+      <c r="A8" s="9">
         <v>7.0</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="11">
+      <c r="B8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="9">
         <v>3.0</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>3.0</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -1257,122 +1257,122 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="22">
+      <c r="A9" s="25">
         <v>8.0</v>
       </c>
-      <c r="B9" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="20" t="s">
+      <c r="B9" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="11">
+      <c r="C9" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="9">
         <v>3.0</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="34">
         <v>6.0</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
+      <c r="A10" s="9">
         <v>9.0</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>13.0</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="32">
+    </row>
+    <row r="11">
+      <c r="A11" s="34">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="34">
         <v>2.0</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E11" s="34">
+        <v>12.0</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="34">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="34">
+        <v>3.0</v>
+      </c>
+      <c r="E12" s="34">
+        <v>11.0</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="34">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="34">
+        <v>2.0</v>
+      </c>
+      <c r="E13" s="34">
+        <v>7.0</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="34">
         <v>13.0</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="32">
-        <v>10.0</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="32">
+      <c r="B14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="34">
         <v>2.0</v>
       </c>
-      <c r="E11" s="32">
-        <v>12.0</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="32">
-        <v>11.0</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="32">
-        <v>3.0</v>
-      </c>
-      <c r="E12" s="32">
-        <v>11.0</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="32">
-        <v>12.0</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="E13" s="32">
-        <v>7.0</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="32">
-        <v>13.0</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="32">
-        <v>2.0</v>
-      </c>
-      <c r="E14" s="32">
+      <c r="E14" s="34">
         <v>4.0</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="11" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1409,35 +1409,35 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="C2" s="5"/>
       <c r="D2" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="C3" s="5"/>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="C4" s="5"/>
       <c r="D4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -1456,58 +1456,58 @@
       <c r="A8" s="7"/>
       <c r="C8" s="5"/>
       <c r="D8" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="7"/>
       <c r="C9" s="5"/>
       <c r="D9" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="7"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
+      <c r="D10" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="7"/>
       <c r="C11" s="5"/>
-      <c r="D11" s="12" t="s">
-        <v>26</v>
+      <c r="D11" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="14" t="s">
-        <v>29</v>
+      <c r="B14" s="15" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="12" t="s">
-        <v>30</v>
+      <c r="B15" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="20" t="s">
-        <v>32</v>
+      <c r="B16" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="20" t="s">
-        <v>46</v>
+      <c r="B17" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="20" t="s">
-        <v>48</v>
+      <c r="B18" s="19" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1534,44 +1534,44 @@
       <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11">
+      <c r="A2" s="9">
         <v>1.0</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="11">
+      <c r="A3" s="9">
         <v>1.0</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>1.0</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="32">
+      <c r="A5" s="34">
         <v>1.0</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -1579,7 +1579,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="32">
+      <c r="A6" s="34">
         <v>1.0</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -1587,45 +1587,45 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="32">
+      <c r="A8" s="34">
         <v>2.0</v>
       </c>
-      <c r="B8" s="12" t="s">
-        <v>90</v>
+      <c r="B8" s="11" t="s">
+        <v>85</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="32">
+      <c r="A9" s="34">
         <v>2.0</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="32">
+      <c r="A10" s="34">
         <v>2.0</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>21</v>
+      <c r="C10" s="11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="32">
+      <c r="A11" s="34">
         <v>2.0</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>26</v>
+      <c r="C11" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="32">
+      <c r="A12" s="34">
         <v>2.0</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1657,38 +1657,38 @@
         <v>81</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D1" s="38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E1" s="38" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F1" s="38" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="39">
         <v>0.0</v>
       </c>
-      <c r="B2" s="40">
+      <c r="B2" s="41">
         <v>42.0</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="41">
         <v>0.0</v>
       </c>
-      <c r="D2" s="40">
+      <c r="D2" s="41">
         <v>0.0</v>
       </c>
-      <c r="E2" s="40">
+      <c r="E2" s="41">
         <v>42.0</v>
       </c>
-      <c r="F2" s="40">
+      <c r="F2" s="41">
         <v>42.0</v>
       </c>
     </row>
@@ -1696,19 +1696,19 @@
       <c r="A3" s="39">
         <v>1.0</v>
       </c>
-      <c r="B3" s="40">
+      <c r="B3" s="41">
         <v>42.0</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="41">
         <v>19.0</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="41">
         <v>19.0</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="41">
         <v>23.0</v>
       </c>
-      <c r="F3" s="40">
+      <c r="F3" s="41">
         <v>23.0</v>
       </c>
     </row>
@@ -1716,19 +1716,19 @@
       <c r="A4" s="39">
         <v>2.0</v>
       </c>
-      <c r="B4" s="40">
+      <c r="B4" s="41">
         <v>42.0</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="41">
         <v>11.0</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="41">
         <v>30.0</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="41">
         <v>12.0</v>
       </c>
-      <c r="F4" s="40">
+      <c r="F4" s="41">
         <v>12.0</v>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
       <c r="A5" s="39">
         <v>3.0</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="41">
         <v>42.0</v>
       </c>
       <c r="C5" s="39"/>

</xml_diff>